<commit_message>
Сreate Excel file according to the example Excel file with importing data from the database.
</commit_message>
<xml_diff>
--- a/Template/example.xlsx
+++ b/Template/example.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASerikov.KGBANK\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Azat\source\repos\Задание\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607FD9AA-3E33-43D9-A0C2-11520767CCEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11985"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>ID:</t>
   </si>
@@ -63,12 +64,15 @@
   </si>
   <si>
     <t>[SocialNumber]</t>
+  </si>
+  <si>
+    <t>[Date]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -560,11 +564,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +587,9 @@
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>

</xml_diff>

<commit_message>
Removed trash from Results directory
</commit_message>
<xml_diff>
--- a/Template/example.xlsx
+++ b/Template/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Azat\source\repos\Задание\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607FD9AA-3E33-43D9-A0C2-11520767CCEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E787AA13-7D86-4289-A6C2-2E4FD454EE4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -568,19 +568,19 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>